<commit_message>
Deciding on nve data to download, cleaning site metadata
</commit_message>
<xml_diff>
--- a/data/NVE/NVE_monitoring_sites.xlsx
+++ b/data/NVE/NVE_monitoring_sites.xlsx
@@ -8,22 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\GitHub\quantom\data\NVE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0D0A248-CC7B-43EF-B70D-D255FAEACDB6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{751A0198-A9B6-4F30-AE07-FD2FC0EBB4CA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MaleserieMalestasjon" sheetId="1" r:id="rId1"/>
+    <sheet name="Selected_for_download" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MaleserieMalestasjon!$A$1:$Y$143</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Selected_for_download!$A$1:$Z$34</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1778" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2268" uniqueCount="275">
   <si>
     <t>objektType</t>
   </si>
@@ -791,6 +793,63 @@
   </si>
   <si>
     <t>Tried downloading, error</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Previously Rappesskaidi, 234.7.0</t>
+  </si>
+  <si>
+    <t>Previously Væhkkava, 234.6.0 (1973 - 1989), located just a few 100m downstream</t>
+  </si>
+  <si>
+    <t>Replaced by Veahkkava</t>
+  </si>
+  <si>
+    <t>Only discharge monitoring on Karasjokha. About 3 km upstream have 2 active stations monitoring water and air temperature and ice thickness</t>
+  </si>
+  <si>
+    <t>Downstream of outflow from Iesjavri lake in NW</t>
+  </si>
+  <si>
+    <t>Old, leave for now, replaced by Jiesjokka</t>
+  </si>
+  <si>
+    <t>Original Polmak station a little downstream (data from 1991-1998, so a crossover between old and new Polmak to help merge data)</t>
+  </si>
+  <si>
+    <t>Small 30 km2'ish catchment that outflows directly to the delta</t>
+  </si>
+  <si>
+    <t>At bridge in Karasjok</t>
+  </si>
+  <si>
+    <t>By Anarjohka</t>
+  </si>
+  <si>
+    <t>2 other stations around Levajok, but very short records. No discharge &amp; discontinued, so probably issues with rating curve</t>
+  </si>
+  <si>
+    <t>Small catchment W of mainstem in N. Only snow data. Just getting in case.</t>
+  </si>
+  <si>
+    <t>Only groundwater data. Small catchment E of mainstem in far N, just before delta (saltwater influence?)</t>
+  </si>
+  <si>
+    <t>Small SC in far NE, by delta. Includes SS and TOC data</t>
+  </si>
+  <si>
+    <t>SS and TOC data. About 20 km US of Polmak</t>
+  </si>
+  <si>
+    <t>Just water temp</t>
+  </si>
+  <si>
+    <t>Replaced by Polmak nye</t>
+  </si>
+  <si>
+    <t>Only version 0, but good location for Anarjohka catchment delineation?</t>
   </si>
 </sst>
 </file>
@@ -850,7 +909,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="2"/>
@@ -859,6 +918,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="2" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1178,10 +1243,10 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:Z143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="Y137" sqref="Y137"/>
+      <selection pane="bottomLeft" activeCell="B13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1204,7 +1269,7 @@
     <col min="24" max="24" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:26">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1280,8 +1345,11 @@
       <c r="Y1" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="2" spans="1:25" hidden="1">
+      <c r="Z1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -1351,8 +1419,11 @@
       <c r="X2">
         <v>69.408237</v>
       </c>
-    </row>
-    <row r="3" spans="1:25" hidden="1">
+      <c r="Y2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" hidden="1">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -1429,7 +1500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:25" hidden="1">
+    <row r="4" spans="1:26">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -1497,7 +1568,7 @@
         <v>69.408237</v>
       </c>
     </row>
-    <row r="5" spans="1:25" hidden="1">
+    <row r="5" spans="1:26" hidden="1">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -1565,7 +1636,7 @@
         <v>69.435312999999994</v>
       </c>
     </row>
-    <row r="6" spans="1:25" hidden="1">
+    <row r="6" spans="1:26" hidden="1">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -1642,7 +1713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:25" hidden="1">
+    <row r="7" spans="1:26" hidden="1">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1715,8 +1786,11 @@
       <c r="X7">
         <v>69.400858999999997</v>
       </c>
-    </row>
-    <row r="8" spans="1:25" hidden="1">
+      <c r="Y7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" hidden="1">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -1790,7 +1864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:25" hidden="1">
+    <row r="9" spans="1:26" hidden="1">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -1861,7 +1935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:25" hidden="1">
+    <row r="10" spans="1:26">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -1929,7 +2003,7 @@
         <v>69.408237</v>
       </c>
     </row>
-    <row r="11" spans="1:25" hidden="1">
+    <row r="11" spans="1:26" hidden="1">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -2002,8 +2076,11 @@
       <c r="X11">
         <v>69.390030999999993</v>
       </c>
-    </row>
-    <row r="12" spans="1:25" hidden="1">
+      <c r="Y11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" hidden="1">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -2073,8 +2150,11 @@
       <c r="X12">
         <v>69.632458999999997</v>
       </c>
-    </row>
-    <row r="13" spans="1:25" hidden="1">
+      <c r="Y12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -2142,10 +2222,10 @@
         <v>69.408237</v>
       </c>
       <c r="Y13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25" hidden="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" hidden="1">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -2213,7 +2293,7 @@
         <v>70.070346999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:25" hidden="1">
+    <row r="15" spans="1:26" hidden="1">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -2287,7 +2367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:25" hidden="1">
+    <row r="16" spans="1:26" hidden="1">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -2429,7 +2509,7 @@
         <v>69.467968999999997</v>
       </c>
     </row>
-    <row r="18" spans="1:25">
+    <row r="18" spans="1:25" hidden="1">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -2573,6 +2653,9 @@
       <c r="X19">
         <v>69.643373999999994</v>
       </c>
+      <c r="Y19">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="1:25" hidden="1">
       <c r="A20" t="s">
@@ -2645,7 +2728,7 @@
         <v>70.399809000000005</v>
       </c>
     </row>
-    <row r="21" spans="1:25">
+    <row r="21" spans="1:25" hidden="1">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -2790,7 +2873,7 @@
         <v>69.564580000000007</v>
       </c>
     </row>
-    <row r="23" spans="1:25">
+    <row r="23" spans="1:25" hidden="1">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -2934,8 +3017,11 @@
       <c r="X24">
         <v>69.665563000000006</v>
       </c>
-    </row>
-    <row r="25" spans="1:25">
+      <c r="Y24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" hidden="1">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -3360,6 +3446,9 @@
       <c r="X30">
         <v>69.688907</v>
       </c>
+      <c r="Y30">
+        <v>0</v>
+      </c>
     </row>
     <row r="31" spans="1:25" hidden="1">
       <c r="A31" t="s">
@@ -3647,6 +3736,9 @@
       <c r="X34">
         <v>69.564580000000007</v>
       </c>
+      <c r="Y34">
+        <v>0</v>
+      </c>
     </row>
     <row r="35" spans="1:25" hidden="1">
       <c r="A35" t="s">
@@ -3863,6 +3955,9 @@
       <c r="X37">
         <v>69.428752000000003</v>
       </c>
+      <c r="Y37">
+        <v>0</v>
+      </c>
     </row>
     <row r="38" spans="1:25" hidden="1">
       <c r="A38" t="s">
@@ -4728,7 +4823,7 @@
         <v>70.072616999999994</v>
       </c>
       <c r="Y49">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:25" hidden="1">
@@ -5162,6 +5257,9 @@
       <c r="X55">
         <v>70.375489999999999</v>
       </c>
+      <c r="Y55">
+        <v>1</v>
+      </c>
     </row>
     <row r="56" spans="1:25" hidden="1">
       <c r="A56" t="s">
@@ -6474,7 +6572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:25">
+    <row r="74" spans="1:25" hidden="1">
       <c r="A74" t="s">
         <v>24</v>
       </c>
@@ -6689,6 +6787,9 @@
       <c r="X76">
         <v>69.469237000000007</v>
       </c>
+      <c r="Y76">
+        <v>1</v>
+      </c>
     </row>
     <row r="77" spans="1:25" hidden="1">
       <c r="A77" t="s">
@@ -6979,8 +7080,11 @@
       <c r="X80">
         <v>69.400755000000004</v>
       </c>
-    </row>
-    <row r="81" spans="1:25" hidden="1">
+      <c r="Y80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:26" hidden="1">
       <c r="A81" t="s">
         <v>24</v>
       </c>
@@ -7054,7 +7158,7 @@
         <v>69.400858999999997</v>
       </c>
     </row>
-    <row r="82" spans="1:25" hidden="1">
+    <row r="82" spans="1:26" hidden="1">
       <c r="A82" t="s">
         <v>24</v>
       </c>
@@ -7128,7 +7232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:25" hidden="1">
+    <row r="83" spans="1:26" hidden="1">
       <c r="A83" t="s">
         <v>24</v>
       </c>
@@ -7202,7 +7306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:25" hidden="1">
+    <row r="84" spans="1:26" hidden="1">
       <c r="A84" t="s">
         <v>24</v>
       </c>
@@ -7270,7 +7374,7 @@
         <v>69.469237000000007</v>
       </c>
     </row>
-    <row r="85" spans="1:25" hidden="1">
+    <row r="85" spans="1:26" hidden="1">
       <c r="A85" t="s">
         <v>24</v>
       </c>
@@ -7344,7 +7448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:25" hidden="1">
+    <row r="86" spans="1:26" hidden="1">
       <c r="A86" t="s">
         <v>24</v>
       </c>
@@ -7414,11 +7518,8 @@
       <c r="X86">
         <v>70.070346999999998</v>
       </c>
-      <c r="Y86">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="1:25" hidden="1">
+    </row>
+    <row r="87" spans="1:26" hidden="1">
       <c r="A87" t="s">
         <v>24</v>
       </c>
@@ -7489,7 +7590,7 @@
         <v>69.435631000000001</v>
       </c>
     </row>
-    <row r="88" spans="1:25" hidden="1">
+    <row r="88" spans="1:26" hidden="1">
       <c r="A88" t="s">
         <v>24</v>
       </c>
@@ -7560,7 +7661,7 @@
         <v>70.079913000000005</v>
       </c>
     </row>
-    <row r="89" spans="1:25" hidden="1">
+    <row r="89" spans="1:26" hidden="1">
       <c r="A89" t="s">
         <v>24</v>
       </c>
@@ -7628,7 +7729,7 @@
         <v>69.438372999999999</v>
       </c>
     </row>
-    <row r="90" spans="1:25" hidden="1">
+    <row r="90" spans="1:26" hidden="1">
       <c r="A90" t="s">
         <v>24</v>
       </c>
@@ -7699,7 +7800,7 @@
         <v>70.166214999999994</v>
       </c>
     </row>
-    <row r="91" spans="1:25" hidden="1">
+    <row r="91" spans="1:26" hidden="1">
       <c r="A91" t="s">
         <v>24</v>
       </c>
@@ -7767,7 +7868,7 @@
         <v>69.407993000000005</v>
       </c>
     </row>
-    <row r="92" spans="1:25" hidden="1">
+    <row r="92" spans="1:26" hidden="1">
       <c r="A92" t="s">
         <v>24</v>
       </c>
@@ -7841,7 +7942,7 @@
         <v>70.070346999999998</v>
       </c>
     </row>
-    <row r="93" spans="1:25" hidden="1">
+    <row r="93" spans="1:26" hidden="1">
       <c r="A93" t="s">
         <v>24</v>
       </c>
@@ -7912,10 +8013,13 @@
         <v>69.619587999999993</v>
       </c>
       <c r="Y93">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="94" spans="1:25" hidden="1">
+        <v>0</v>
+      </c>
+      <c r="Z93" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="94" spans="1:26" hidden="1">
       <c r="A94" t="s">
         <v>24</v>
       </c>
@@ -7986,7 +8090,7 @@
         <v>70.166214999999994</v>
       </c>
     </row>
-    <row r="95" spans="1:25" hidden="1">
+    <row r="95" spans="1:26" hidden="1">
       <c r="A95" t="s">
         <v>24</v>
       </c>
@@ -8053,8 +8157,11 @@
       <c r="X95">
         <v>69.435631000000001</v>
       </c>
-    </row>
-    <row r="96" spans="1:25" hidden="1">
+      <c r="Y95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:26" hidden="1">
       <c r="A96" t="s">
         <v>24</v>
       </c>
@@ -8195,6 +8302,9 @@
       <c r="X97">
         <v>70.074292</v>
       </c>
+      <c r="Y97">
+        <v>1</v>
+      </c>
     </row>
     <row r="98" spans="1:26" hidden="1">
       <c r="A98" t="s">
@@ -8473,6 +8583,9 @@
       <c r="X101">
         <v>69.407993000000005</v>
       </c>
+      <c r="Y101">
+        <v>0</v>
+      </c>
     </row>
     <row r="102" spans="1:26" hidden="1">
       <c r="A102" t="s">
@@ -8545,7 +8658,7 @@
         <v>70.070346999999998</v>
       </c>
     </row>
-    <row r="103" spans="1:26">
+    <row r="103" spans="1:26" hidden="1">
       <c r="A103" t="s">
         <v>24</v>
       </c>
@@ -8689,6 +8802,9 @@
       <c r="X104">
         <v>69.400858999999997</v>
       </c>
+      <c r="Y104">
+        <v>1</v>
+      </c>
     </row>
     <row r="105" spans="1:26" hidden="1">
       <c r="A105" t="s">
@@ -8977,7 +9093,7 @@
         <v>69.400685999999993</v>
       </c>
       <c r="Y108">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="109" spans="1:26" hidden="1">
@@ -9057,7 +9173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:26">
+    <row r="110" spans="1:26" hidden="1">
       <c r="A110" t="s">
         <v>24</v>
       </c>
@@ -9417,6 +9533,9 @@
       <c r="X114">
         <v>69.944618000000006</v>
       </c>
+      <c r="Y114">
+        <v>0</v>
+      </c>
     </row>
     <row r="115" spans="1:25" hidden="1">
       <c r="A115" t="s">
@@ -9643,7 +9762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:25">
+    <row r="118" spans="1:25" hidden="1">
       <c r="A118" t="s">
         <v>24</v>
       </c>
@@ -9787,6 +9906,9 @@
       <c r="X119">
         <v>70.061885000000004</v>
       </c>
+      <c r="Y119">
+        <v>0</v>
+      </c>
     </row>
     <row r="120" spans="1:25" hidden="1">
       <c r="A120" t="s">
@@ -10074,6 +10196,9 @@
       <c r="X123">
         <v>70.070637000000005</v>
       </c>
+      <c r="Y123">
+        <v>1</v>
+      </c>
     </row>
     <row r="124" spans="1:25" hidden="1">
       <c r="A124" t="s">
@@ -10214,7 +10339,7 @@
         <v>70.070346999999998</v>
       </c>
     </row>
-    <row r="126" spans="1:25">
+    <row r="126" spans="1:25" hidden="1">
       <c r="A126" t="s">
         <v>24</v>
       </c>
@@ -10648,6 +10773,9 @@
       <c r="X131">
         <v>70.012997999999996</v>
       </c>
+      <c r="Y131">
+        <v>0</v>
+      </c>
     </row>
     <row r="132" spans="1:25" hidden="1">
       <c r="A132" t="s">
@@ -10790,6 +10918,9 @@
       <c r="X133">
         <v>69.426393000000004</v>
       </c>
+      <c r="Y133">
+        <v>1</v>
+      </c>
     </row>
     <row r="134" spans="1:25" hidden="1">
       <c r="A134" t="s">
@@ -10861,6 +10992,9 @@
       <c r="X134">
         <v>69.886965000000004</v>
       </c>
+      <c r="Y134">
+        <v>0</v>
+      </c>
     </row>
     <row r="135" spans="1:25" hidden="1">
       <c r="A135" t="s">
@@ -11010,7 +11144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:25">
+    <row r="137" spans="1:25" hidden="1">
       <c r="A137" s="2" t="s">
         <v>24</v>
       </c>
@@ -11533,14 +11667,15 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:Y143" xr:uid="{A6326A3A-6B72-4363-90F2-C3D336D85C53}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="Anarjokka ovf. Karasjokka"/>
+      </filters>
+    </filterColumn>
     <filterColumn colId="6">
       <filters>
-        <filter val="Vannføring"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="10">
-      <filters>
-        <filter val="1"/>
+        <filter val="Grunnvannsnivå"/>
+        <filter val="Vanntemperatur"/>
       </filters>
     </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Y134">
@@ -11549,4 +11684,2751 @@
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9712F67-37DA-4684-928B-6119F2A35904}">
+  <dimension ref="A1:Z35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>247</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E2">
+        <v>6</v>
+      </c>
+      <c r="F2">
+        <v>1003</v>
+      </c>
+      <c r="G2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" t="s">
+        <v>105</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>30</v>
+      </c>
+      <c r="M2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N2">
+        <v>2190</v>
+      </c>
+      <c r="O2" t="s">
+        <v>106</v>
+      </c>
+      <c r="P2" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q2">
+        <v>22</v>
+      </c>
+      <c r="R2">
+        <v>20160527</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2" s="1">
+        <v>44573</v>
+      </c>
+      <c r="U2" t="s">
+        <v>33</v>
+      </c>
+      <c r="V2" t="s">
+        <v>34</v>
+      </c>
+      <c r="W2">
+        <v>24.474238</v>
+      </c>
+      <c r="X2">
+        <v>69.390030999999993</v>
+      </c>
+      <c r="Y2">
+        <v>1</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E3">
+        <v>8</v>
+      </c>
+      <c r="F3">
+        <v>1001</v>
+      </c>
+      <c r="G3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>39</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>30</v>
+      </c>
+      <c r="M3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N3">
+        <v>2190</v>
+      </c>
+      <c r="O3" t="s">
+        <v>106</v>
+      </c>
+      <c r="P3" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q3">
+        <v>22</v>
+      </c>
+      <c r="R3">
+        <v>19780130</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3" s="1">
+        <v>44573</v>
+      </c>
+      <c r="U3" t="s">
+        <v>33</v>
+      </c>
+      <c r="V3" t="s">
+        <v>34</v>
+      </c>
+      <c r="W3">
+        <v>24.474238</v>
+      </c>
+      <c r="X3">
+        <v>69.390030999999993</v>
+      </c>
+      <c r="Y3">
+        <v>1</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C4" t="s">
+        <v>164</v>
+      </c>
+      <c r="D4" t="s">
+        <v>165</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>2000</v>
+      </c>
+      <c r="G4" t="s">
+        <v>83</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4" t="s">
+        <v>39</v>
+      </c>
+      <c r="J4" t="s">
+        <v>58</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4" t="s">
+        <v>30</v>
+      </c>
+      <c r="M4" t="s">
+        <v>30</v>
+      </c>
+      <c r="N4" t="s">
+        <v>30</v>
+      </c>
+      <c r="O4" t="s">
+        <v>166</v>
+      </c>
+      <c r="P4" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q4">
+        <v>22</v>
+      </c>
+      <c r="R4">
+        <v>20010807</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4" s="1">
+        <v>44573</v>
+      </c>
+      <c r="U4" t="s">
+        <v>33</v>
+      </c>
+      <c r="V4" t="s">
+        <v>34</v>
+      </c>
+      <c r="W4">
+        <v>28.249378</v>
+      </c>
+      <c r="X4">
+        <v>70.375489999999999</v>
+      </c>
+      <c r="Y4">
+        <v>1</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>163</v>
+      </c>
+      <c r="C5" t="s">
+        <v>164</v>
+      </c>
+      <c r="D5" t="s">
+        <v>165</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>2015</v>
+      </c>
+      <c r="G5" t="s">
+        <v>57</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" t="s">
+        <v>58</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5" t="s">
+        <v>30</v>
+      </c>
+      <c r="M5" t="s">
+        <v>30</v>
+      </c>
+      <c r="N5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O5" t="s">
+        <v>166</v>
+      </c>
+      <c r="P5" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q5">
+        <v>22</v>
+      </c>
+      <c r="R5">
+        <v>20010807</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5" s="1">
+        <v>44573</v>
+      </c>
+      <c r="U5" t="s">
+        <v>33</v>
+      </c>
+      <c r="V5" t="s">
+        <v>34</v>
+      </c>
+      <c r="W5">
+        <v>28.249378</v>
+      </c>
+      <c r="X5">
+        <v>70.375489999999999</v>
+      </c>
+      <c r="Y5">
+        <v>1</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>110</v>
+      </c>
+      <c r="C6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D6" t="s">
+        <v>112</v>
+      </c>
+      <c r="E6">
+        <v>8</v>
+      </c>
+      <c r="F6">
+        <v>1001</v>
+      </c>
+      <c r="G6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="J6" t="s">
+        <v>113</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6" t="s">
+        <v>30</v>
+      </c>
+      <c r="M6" t="s">
+        <v>30</v>
+      </c>
+      <c r="N6">
+        <v>2181</v>
+      </c>
+      <c r="O6" t="s">
+        <v>71</v>
+      </c>
+      <c r="P6" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q6">
+        <v>22</v>
+      </c>
+      <c r="R6">
+        <v>19570715</v>
+      </c>
+      <c r="S6">
+        <v>19820726</v>
+      </c>
+      <c r="T6" s="1">
+        <v>44573</v>
+      </c>
+      <c r="U6" t="s">
+        <v>33</v>
+      </c>
+      <c r="V6" t="s">
+        <v>34</v>
+      </c>
+      <c r="W6">
+        <v>24.388183000000001</v>
+      </c>
+      <c r="X6">
+        <v>69.565611000000004</v>
+      </c>
+      <c r="Y6">
+        <v>1</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26">
+      <c r="A7" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="E7" s="8">
+        <v>8</v>
+      </c>
+      <c r="F7" s="8">
+        <v>1001</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="H7" s="8">
+        <v>0</v>
+      </c>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="K7" s="8">
+        <v>1</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="M7" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="N7" s="8">
+        <v>2192</v>
+      </c>
+      <c r="O7" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="P7" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="Q7" s="8">
+        <v>22</v>
+      </c>
+      <c r="R7" s="8">
+        <v>19910915</v>
+      </c>
+      <c r="S7" s="8">
+        <v>20040322</v>
+      </c>
+      <c r="T7" s="11">
+        <v>44573</v>
+      </c>
+      <c r="U7" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="V7" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="W7" s="8">
+        <v>28.824532000000001</v>
+      </c>
+      <c r="X7" s="8">
+        <v>70.472215000000006</v>
+      </c>
+      <c r="Y7" s="12">
+        <v>1</v>
+      </c>
+      <c r="Z7" s="2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26">
+      <c r="A8" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="E8" s="8">
+        <v>4</v>
+      </c>
+      <c r="F8" s="8">
+        <v>1208</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="H8" s="8">
+        <v>0</v>
+      </c>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="K8" s="8">
+        <v>1</v>
+      </c>
+      <c r="L8" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="M8" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="N8" s="8">
+        <v>2192</v>
+      </c>
+      <c r="O8" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="P8" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="Q8" s="8">
+        <v>22</v>
+      </c>
+      <c r="R8" s="8">
+        <v>19910925</v>
+      </c>
+      <c r="S8" s="8">
+        <v>19970625</v>
+      </c>
+      <c r="T8" s="10">
+        <v>44573</v>
+      </c>
+      <c r="U8" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="V8" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="W8" s="8">
+        <v>28.824532000000001</v>
+      </c>
+      <c r="X8" s="8">
+        <v>70.472215000000006</v>
+      </c>
+      <c r="Y8" s="12">
+        <v>1</v>
+      </c>
+      <c r="Z8" s="2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26">
+      <c r="A9" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="E9" s="8">
+        <v>4</v>
+      </c>
+      <c r="F9" s="8">
+        <v>1200</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="H9" s="8">
+        <v>0</v>
+      </c>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="K9" s="8">
+        <v>1</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="M9" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="N9" s="8">
+        <v>2192</v>
+      </c>
+      <c r="O9" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="P9" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="Q9" s="8">
+        <v>22</v>
+      </c>
+      <c r="R9" s="8">
+        <v>19910925</v>
+      </c>
+      <c r="S9" s="8">
+        <v>19970625</v>
+      </c>
+      <c r="T9" s="10">
+        <v>44573</v>
+      </c>
+      <c r="U9" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="V9" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="W9" s="8">
+        <v>28.824532000000001</v>
+      </c>
+      <c r="X9" s="8">
+        <v>70.472215000000006</v>
+      </c>
+      <c r="Y9" s="12">
+        <v>1</v>
+      </c>
+      <c r="Z9" s="2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>114</v>
+      </c>
+      <c r="C10" t="s">
+        <v>115</v>
+      </c>
+      <c r="D10" t="s">
+        <v>116</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1000</v>
+      </c>
+      <c r="G10" t="s">
+        <v>62</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="J10" t="s">
+        <v>29</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10" t="s">
+        <v>30</v>
+      </c>
+      <c r="M10" t="s">
+        <v>30</v>
+      </c>
+      <c r="N10">
+        <v>2349</v>
+      </c>
+      <c r="O10" t="s">
+        <v>117</v>
+      </c>
+      <c r="P10" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q10">
+        <v>22</v>
+      </c>
+      <c r="R10">
+        <v>19980331</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10" s="1">
+        <v>44573</v>
+      </c>
+      <c r="U10" t="s">
+        <v>33</v>
+      </c>
+      <c r="V10" t="s">
+        <v>34</v>
+      </c>
+      <c r="W10">
+        <v>25.510739000000001</v>
+      </c>
+      <c r="X10">
+        <v>69.469237000000007</v>
+      </c>
+      <c r="Y10">
+        <v>1</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" t="s">
+        <v>114</v>
+      </c>
+      <c r="C11" t="s">
+        <v>115</v>
+      </c>
+      <c r="D11" t="s">
+        <v>116</v>
+      </c>
+      <c r="E11">
+        <v>6</v>
+      </c>
+      <c r="F11">
+        <v>1003</v>
+      </c>
+      <c r="G11" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="J11" t="s">
+        <v>29</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11" t="s">
+        <v>30</v>
+      </c>
+      <c r="M11" t="s">
+        <v>30</v>
+      </c>
+      <c r="N11">
+        <v>2349</v>
+      </c>
+      <c r="O11" t="s">
+        <v>117</v>
+      </c>
+      <c r="P11" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q11">
+        <v>22</v>
+      </c>
+      <c r="R11">
+        <v>19981025</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11" s="1">
+        <v>44573</v>
+      </c>
+      <c r="U11" t="s">
+        <v>33</v>
+      </c>
+      <c r="V11" t="s">
+        <v>34</v>
+      </c>
+      <c r="W11">
+        <v>25.510739000000001</v>
+      </c>
+      <c r="X11">
+        <v>69.469237000000007</v>
+      </c>
+      <c r="Y11">
+        <v>1</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
+        <v>206</v>
+      </c>
+      <c r="C12" t="s">
+        <v>207</v>
+      </c>
+      <c r="D12" t="s">
+        <v>208</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
+      <c r="F12">
+        <v>2000</v>
+      </c>
+      <c r="G12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="J12" t="s">
+        <v>58</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12" t="s">
+        <v>30</v>
+      </c>
+      <c r="M12" t="s">
+        <v>30</v>
+      </c>
+      <c r="N12" t="s">
+        <v>30</v>
+      </c>
+      <c r="O12" t="s">
+        <v>41</v>
+      </c>
+      <c r="P12" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q12">
+        <v>22</v>
+      </c>
+      <c r="R12">
+        <v>19810114</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+      <c r="T12" s="1">
+        <v>44573</v>
+      </c>
+      <c r="U12" t="s">
+        <v>33</v>
+      </c>
+      <c r="V12" t="s">
+        <v>34</v>
+      </c>
+      <c r="W12">
+        <v>25.815045999999999</v>
+      </c>
+      <c r="X12">
+        <v>69.400755000000004</v>
+      </c>
+      <c r="Y12">
+        <v>1</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>206</v>
+      </c>
+      <c r="C13" t="s">
+        <v>207</v>
+      </c>
+      <c r="D13" t="s">
+        <v>208</v>
+      </c>
+      <c r="E13">
+        <v>3</v>
+      </c>
+      <c r="F13">
+        <v>2015</v>
+      </c>
+      <c r="G13" t="s">
+        <v>57</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="J13" t="s">
+        <v>58</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="L13" t="s">
+        <v>30</v>
+      </c>
+      <c r="M13" t="s">
+        <v>30</v>
+      </c>
+      <c r="N13" t="s">
+        <v>30</v>
+      </c>
+      <c r="O13" t="s">
+        <v>41</v>
+      </c>
+      <c r="P13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q13">
+        <v>22</v>
+      </c>
+      <c r="R13">
+        <v>19820824</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+      <c r="T13" s="1">
+        <v>44573</v>
+      </c>
+      <c r="U13" t="s">
+        <v>33</v>
+      </c>
+      <c r="V13" t="s">
+        <v>34</v>
+      </c>
+      <c r="W13">
+        <v>25.815045999999999</v>
+      </c>
+      <c r="X13">
+        <v>69.400755000000004</v>
+      </c>
+      <c r="Y13">
+        <v>1</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" t="s">
+        <v>180</v>
+      </c>
+      <c r="C14" t="s">
+        <v>181</v>
+      </c>
+      <c r="D14" t="s">
+        <v>182</v>
+      </c>
+      <c r="E14">
+        <v>3</v>
+      </c>
+      <c r="F14">
+        <v>2000</v>
+      </c>
+      <c r="G14" t="s">
+        <v>83</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="J14" t="s">
+        <v>58</v>
+      </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="L14" t="s">
+        <v>30</v>
+      </c>
+      <c r="M14" t="s">
+        <v>30</v>
+      </c>
+      <c r="N14" t="s">
+        <v>30</v>
+      </c>
+      <c r="O14" t="s">
+        <v>41</v>
+      </c>
+      <c r="P14" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q14">
+        <v>22</v>
+      </c>
+      <c r="R14">
+        <v>19810130</v>
+      </c>
+      <c r="S14">
+        <v>19901231</v>
+      </c>
+      <c r="T14" s="1">
+        <v>44573</v>
+      </c>
+      <c r="U14" t="s">
+        <v>33</v>
+      </c>
+      <c r="V14" t="s">
+        <v>34</v>
+      </c>
+      <c r="W14">
+        <v>25.814402000000001</v>
+      </c>
+      <c r="X14">
+        <v>69.400858999999997</v>
+      </c>
+      <c r="Y14">
+        <v>1</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15">
+        <v>3</v>
+      </c>
+      <c r="F15">
+        <v>2006</v>
+      </c>
+      <c r="G15" t="s">
+        <v>38</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15" t="s">
+        <v>39</v>
+      </c>
+      <c r="J15" t="s">
+        <v>40</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15" t="s">
+        <v>30</v>
+      </c>
+      <c r="M15" t="s">
+        <v>30</v>
+      </c>
+      <c r="N15" t="s">
+        <v>30</v>
+      </c>
+      <c r="O15" t="s">
+        <v>41</v>
+      </c>
+      <c r="P15" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q15">
+        <v>22</v>
+      </c>
+      <c r="R15">
+        <v>20050726</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15" s="1">
+        <v>44573</v>
+      </c>
+      <c r="U15" t="s">
+        <v>33</v>
+      </c>
+      <c r="V15" t="s">
+        <v>34</v>
+      </c>
+      <c r="W15">
+        <v>25.814402000000001</v>
+      </c>
+      <c r="X15">
+        <v>69.400858999999997</v>
+      </c>
+      <c r="Y15">
+        <v>1</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16">
+        <v>3</v>
+      </c>
+      <c r="F16">
+        <v>2015</v>
+      </c>
+      <c r="G16" t="s">
+        <v>57</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16" t="s">
+        <v>39</v>
+      </c>
+      <c r="J16" t="s">
+        <v>58</v>
+      </c>
+      <c r="K16">
+        <v>1</v>
+      </c>
+      <c r="L16" t="s">
+        <v>30</v>
+      </c>
+      <c r="M16" t="s">
+        <v>30</v>
+      </c>
+      <c r="N16" t="s">
+        <v>30</v>
+      </c>
+      <c r="O16" t="s">
+        <v>41</v>
+      </c>
+      <c r="P16" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q16">
+        <v>22</v>
+      </c>
+      <c r="R16">
+        <v>20040923</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+      <c r="T16" s="1">
+        <v>44573</v>
+      </c>
+      <c r="U16" t="s">
+        <v>33</v>
+      </c>
+      <c r="V16" t="s">
+        <v>34</v>
+      </c>
+      <c r="W16">
+        <v>25.814402000000001</v>
+      </c>
+      <c r="X16">
+        <v>69.400858999999997</v>
+      </c>
+      <c r="Y16">
+        <v>1</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17">
+        <v>3</v>
+      </c>
+      <c r="F17">
+        <v>2001</v>
+      </c>
+      <c r="G17" t="s">
+        <v>233</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="J17" t="s">
+        <v>40</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="L17" t="s">
+        <v>30</v>
+      </c>
+      <c r="M17" t="s">
+        <v>30</v>
+      </c>
+      <c r="N17" t="s">
+        <v>30</v>
+      </c>
+      <c r="O17" t="s">
+        <v>41</v>
+      </c>
+      <c r="P17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q17">
+        <v>22</v>
+      </c>
+      <c r="R17">
+        <v>20060629</v>
+      </c>
+      <c r="S17">
+        <v>0</v>
+      </c>
+      <c r="T17" s="1">
+        <v>44573</v>
+      </c>
+      <c r="U17" t="s">
+        <v>33</v>
+      </c>
+      <c r="V17" t="s">
+        <v>34</v>
+      </c>
+      <c r="W17">
+        <v>25.814402000000001</v>
+      </c>
+      <c r="X17">
+        <v>69.400858999999997</v>
+      </c>
+      <c r="Y17">
+        <v>1</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26">
+      <c r="A18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18">
+        <v>3</v>
+      </c>
+      <c r="F18">
+        <v>2000</v>
+      </c>
+      <c r="G18" t="s">
+        <v>83</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18" t="s">
+        <v>39</v>
+      </c>
+      <c r="J18" t="s">
+        <v>58</v>
+      </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="L18" t="s">
+        <v>30</v>
+      </c>
+      <c r="M18" t="s">
+        <v>30</v>
+      </c>
+      <c r="N18" t="s">
+        <v>30</v>
+      </c>
+      <c r="O18" t="s">
+        <v>41</v>
+      </c>
+      <c r="P18" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q18">
+        <v>22</v>
+      </c>
+      <c r="R18">
+        <v>20040710</v>
+      </c>
+      <c r="S18">
+        <v>0</v>
+      </c>
+      <c r="T18" s="1">
+        <v>44573</v>
+      </c>
+      <c r="U18" t="s">
+        <v>33</v>
+      </c>
+      <c r="V18" t="s">
+        <v>34</v>
+      </c>
+      <c r="W18">
+        <v>25.814402000000001</v>
+      </c>
+      <c r="X18">
+        <v>69.400858999999997</v>
+      </c>
+      <c r="Y18">
+        <v>1</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26">
+      <c r="A19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" t="s">
+        <v>169</v>
+      </c>
+      <c r="C19" t="s">
+        <v>170</v>
+      </c>
+      <c r="D19" t="s">
+        <v>171</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>1000</v>
+      </c>
+      <c r="G19" t="s">
+        <v>62</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="J19" t="s">
+        <v>29</v>
+      </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="L19" t="s">
+        <v>30</v>
+      </c>
+      <c r="M19" t="s">
+        <v>30</v>
+      </c>
+      <c r="N19">
+        <v>2188</v>
+      </c>
+      <c r="O19" t="s">
+        <v>172</v>
+      </c>
+      <c r="P19" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q19">
+        <v>22</v>
+      </c>
+      <c r="R19">
+        <v>19980331</v>
+      </c>
+      <c r="S19">
+        <v>20050312</v>
+      </c>
+      <c r="T19" s="1">
+        <v>44573</v>
+      </c>
+      <c r="U19" t="s">
+        <v>33</v>
+      </c>
+      <c r="V19" t="s">
+        <v>34</v>
+      </c>
+      <c r="W19">
+        <v>26.485793000000001</v>
+      </c>
+      <c r="X19">
+        <v>69.944618000000006</v>
+      </c>
+      <c r="Y19">
+        <v>1</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26">
+      <c r="A20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" t="s">
+        <v>156</v>
+      </c>
+      <c r="C20" t="s">
+        <v>157</v>
+      </c>
+      <c r="D20" t="s">
+        <v>158</v>
+      </c>
+      <c r="E20">
+        <v>8</v>
+      </c>
+      <c r="F20">
+        <v>1001</v>
+      </c>
+      <c r="G20" t="s">
+        <v>54</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="J20" t="s">
+        <v>113</v>
+      </c>
+      <c r="K20">
+        <v>1</v>
+      </c>
+      <c r="L20" t="s">
+        <v>30</v>
+      </c>
+      <c r="M20" t="s">
+        <v>30</v>
+      </c>
+      <c r="N20">
+        <v>2184</v>
+      </c>
+      <c r="O20" t="s">
+        <v>46</v>
+      </c>
+      <c r="P20" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q20">
+        <v>22</v>
+      </c>
+      <c r="R20">
+        <v>19661006</v>
+      </c>
+      <c r="S20">
+        <v>19910817</v>
+      </c>
+      <c r="T20" s="1">
+        <v>44573</v>
+      </c>
+      <c r="U20" t="s">
+        <v>33</v>
+      </c>
+      <c r="V20" t="s">
+        <v>34</v>
+      </c>
+      <c r="W20">
+        <v>25.158322999999999</v>
+      </c>
+      <c r="X20">
+        <v>69.419317000000007</v>
+      </c>
+      <c r="Y20">
+        <v>1</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" t="s">
+        <v>85</v>
+      </c>
+      <c r="C21" t="s">
+        <v>86</v>
+      </c>
+      <c r="D21" t="s">
+        <v>87</v>
+      </c>
+      <c r="E21">
+        <v>8</v>
+      </c>
+      <c r="F21">
+        <v>1001</v>
+      </c>
+      <c r="G21" t="s">
+        <v>54</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>1</v>
+      </c>
+      <c r="L21" t="s">
+        <v>30</v>
+      </c>
+      <c r="M21" t="s">
+        <v>30</v>
+      </c>
+      <c r="N21">
+        <v>2180</v>
+      </c>
+      <c r="O21" t="s">
+        <v>89</v>
+      </c>
+      <c r="P21" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q21">
+        <v>22</v>
+      </c>
+      <c r="R21">
+        <v>19110724</v>
+      </c>
+      <c r="S21">
+        <v>19980118</v>
+      </c>
+      <c r="T21" s="1">
+        <v>44573</v>
+      </c>
+      <c r="U21" t="s">
+        <v>33</v>
+      </c>
+      <c r="V21" t="s">
+        <v>34</v>
+      </c>
+      <c r="W21">
+        <v>28.057406</v>
+      </c>
+      <c r="X21">
+        <v>70.072616999999994</v>
+      </c>
+      <c r="Y21">
+        <v>1</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22" t="s">
+        <v>66</v>
+      </c>
+      <c r="E22">
+        <v>4</v>
+      </c>
+      <c r="F22">
+        <v>1200</v>
+      </c>
+      <c r="G22" t="s">
+        <v>88</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="J22" t="s">
+        <v>29</v>
+      </c>
+      <c r="K22">
+        <v>1</v>
+      </c>
+      <c r="L22" t="s">
+        <v>30</v>
+      </c>
+      <c r="M22" t="s">
+        <v>30</v>
+      </c>
+      <c r="N22">
+        <v>2194</v>
+      </c>
+      <c r="O22" t="s">
+        <v>63</v>
+      </c>
+      <c r="P22" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q22">
+        <v>22</v>
+      </c>
+      <c r="R22">
+        <v>19990619</v>
+      </c>
+      <c r="S22">
+        <v>0</v>
+      </c>
+      <c r="T22" s="1">
+        <v>44573</v>
+      </c>
+      <c r="U22" t="s">
+        <v>33</v>
+      </c>
+      <c r="V22" t="s">
+        <v>34</v>
+      </c>
+      <c r="W22">
+        <v>28.016017000000002</v>
+      </c>
+      <c r="X22">
+        <v>70.070346999999998</v>
+      </c>
+      <c r="Y22">
+        <v>1</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" t="s">
+        <v>65</v>
+      </c>
+      <c r="D23" t="s">
+        <v>66</v>
+      </c>
+      <c r="E23">
+        <v>4</v>
+      </c>
+      <c r="F23">
+        <v>1208</v>
+      </c>
+      <c r="G23" t="s">
+        <v>179</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="J23" t="s">
+        <v>29</v>
+      </c>
+      <c r="K23">
+        <v>1</v>
+      </c>
+      <c r="L23" t="s">
+        <v>30</v>
+      </c>
+      <c r="M23" t="s">
+        <v>30</v>
+      </c>
+      <c r="N23">
+        <v>2194</v>
+      </c>
+      <c r="O23" t="s">
+        <v>63</v>
+      </c>
+      <c r="P23" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q23">
+        <v>22</v>
+      </c>
+      <c r="R23">
+        <v>19990619</v>
+      </c>
+      <c r="S23">
+        <v>0</v>
+      </c>
+      <c r="T23" s="1">
+        <v>44573</v>
+      </c>
+      <c r="U23" t="s">
+        <v>33</v>
+      </c>
+      <c r="V23" t="s">
+        <v>34</v>
+      </c>
+      <c r="W23">
+        <v>28.016017000000002</v>
+      </c>
+      <c r="X23">
+        <v>70.070346999999998</v>
+      </c>
+      <c r="Y23">
+        <v>1</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" t="s">
+        <v>64</v>
+      </c>
+      <c r="C24" t="s">
+        <v>65</v>
+      </c>
+      <c r="D24" t="s">
+        <v>66</v>
+      </c>
+      <c r="E24">
+        <v>8</v>
+      </c>
+      <c r="F24">
+        <v>1001</v>
+      </c>
+      <c r="G24" t="s">
+        <v>54</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="I24" t="s">
+        <v>39</v>
+      </c>
+      <c r="K24">
+        <v>1</v>
+      </c>
+      <c r="L24" t="s">
+        <v>30</v>
+      </c>
+      <c r="M24" t="s">
+        <v>30</v>
+      </c>
+      <c r="N24">
+        <v>2194</v>
+      </c>
+      <c r="O24" t="s">
+        <v>63</v>
+      </c>
+      <c r="P24" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q24">
+        <v>22</v>
+      </c>
+      <c r="R24">
+        <v>19911201</v>
+      </c>
+      <c r="S24">
+        <v>0</v>
+      </c>
+      <c r="T24" s="1">
+        <v>44573</v>
+      </c>
+      <c r="U24" t="s">
+        <v>33</v>
+      </c>
+      <c r="V24" t="s">
+        <v>34</v>
+      </c>
+      <c r="W24">
+        <v>28.016017000000002</v>
+      </c>
+      <c r="X24">
+        <v>70.070346999999998</v>
+      </c>
+      <c r="Y24">
+        <v>1</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>64</v>
+      </c>
+      <c r="C25" t="s">
+        <v>65</v>
+      </c>
+      <c r="D25" t="s">
+        <v>66</v>
+      </c>
+      <c r="E25">
+        <v>6</v>
+      </c>
+      <c r="F25">
+        <v>1003</v>
+      </c>
+      <c r="G25" t="s">
+        <v>28</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="I25" t="s">
+        <v>39</v>
+      </c>
+      <c r="J25" t="s">
+        <v>29</v>
+      </c>
+      <c r="K25">
+        <v>1</v>
+      </c>
+      <c r="L25" t="s">
+        <v>30</v>
+      </c>
+      <c r="M25" t="s">
+        <v>30</v>
+      </c>
+      <c r="N25">
+        <v>2194</v>
+      </c>
+      <c r="O25" t="s">
+        <v>63</v>
+      </c>
+      <c r="P25" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q25">
+        <v>22</v>
+      </c>
+      <c r="R25">
+        <v>20071012</v>
+      </c>
+      <c r="S25">
+        <v>0</v>
+      </c>
+      <c r="T25" s="1">
+        <v>44573</v>
+      </c>
+      <c r="U25" t="s">
+        <v>33</v>
+      </c>
+      <c r="V25" t="s">
+        <v>34</v>
+      </c>
+      <c r="W25">
+        <v>28.016017000000002</v>
+      </c>
+      <c r="X25">
+        <v>70.070346999999998</v>
+      </c>
+      <c r="Y25">
+        <v>1</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26">
+      <c r="A26" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>173</v>
+      </c>
+      <c r="C26" t="s">
+        <v>174</v>
+      </c>
+      <c r="D26" t="s">
+        <v>175</v>
+      </c>
+      <c r="E26">
+        <v>5</v>
+      </c>
+      <c r="F26">
+        <v>2002</v>
+      </c>
+      <c r="G26" t="s">
+        <v>176</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26" t="s">
+        <v>39</v>
+      </c>
+      <c r="J26" t="s">
+        <v>177</v>
+      </c>
+      <c r="K26">
+        <v>1</v>
+      </c>
+      <c r="L26" t="s">
+        <v>30</v>
+      </c>
+      <c r="M26" t="s">
+        <v>30</v>
+      </c>
+      <c r="N26" t="s">
+        <v>30</v>
+      </c>
+      <c r="O26" t="s">
+        <v>178</v>
+      </c>
+      <c r="P26" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q26">
+        <v>28</v>
+      </c>
+      <c r="R26">
+        <v>20100905</v>
+      </c>
+      <c r="S26">
+        <v>20120522</v>
+      </c>
+      <c r="T26" s="1">
+        <v>44573</v>
+      </c>
+      <c r="U26" t="s">
+        <v>33</v>
+      </c>
+      <c r="V26" t="s">
+        <v>34</v>
+      </c>
+      <c r="W26">
+        <v>28.22343</v>
+      </c>
+      <c r="X26">
+        <v>70.166214999999994</v>
+      </c>
+      <c r="Y26">
+        <v>1</v>
+      </c>
+      <c r="Z26" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26">
+      <c r="A27" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" t="s">
+        <v>234</v>
+      </c>
+      <c r="C27" t="s">
+        <v>235</v>
+      </c>
+      <c r="D27" t="s">
+        <v>236</v>
+      </c>
+      <c r="E27">
+        <v>8</v>
+      </c>
+      <c r="F27">
+        <v>1001</v>
+      </c>
+      <c r="G27" t="s">
+        <v>54</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="J27" t="s">
+        <v>113</v>
+      </c>
+      <c r="K27">
+        <v>1</v>
+      </c>
+      <c r="L27" t="s">
+        <v>30</v>
+      </c>
+      <c r="M27" t="s">
+        <v>30</v>
+      </c>
+      <c r="N27">
+        <v>2183</v>
+      </c>
+      <c r="O27" t="s">
+        <v>237</v>
+      </c>
+      <c r="P27" t="s">
+        <v>238</v>
+      </c>
+      <c r="Q27">
+        <v>22</v>
+      </c>
+      <c r="R27">
+        <v>19600803</v>
+      </c>
+      <c r="S27">
+        <v>19910823</v>
+      </c>
+      <c r="T27" s="1">
+        <v>44573</v>
+      </c>
+      <c r="U27" t="s">
+        <v>33</v>
+      </c>
+      <c r="V27" t="s">
+        <v>34</v>
+      </c>
+      <c r="W27">
+        <v>28.041376</v>
+      </c>
+      <c r="X27">
+        <v>70.419150999999999</v>
+      </c>
+      <c r="Y27">
+        <v>1</v>
+      </c>
+      <c r="Z27" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26">
+      <c r="A28" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" t="s">
+        <v>227</v>
+      </c>
+      <c r="C28" t="s">
+        <v>228</v>
+      </c>
+      <c r="D28" t="s">
+        <v>229</v>
+      </c>
+      <c r="E28">
+        <v>6</v>
+      </c>
+      <c r="F28">
+        <v>1003</v>
+      </c>
+      <c r="G28" t="s">
+        <v>28</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="J28" t="s">
+        <v>29</v>
+      </c>
+      <c r="K28">
+        <v>1</v>
+      </c>
+      <c r="L28" t="s">
+        <v>30</v>
+      </c>
+      <c r="M28" t="s">
+        <v>30</v>
+      </c>
+      <c r="N28" t="s">
+        <v>30</v>
+      </c>
+      <c r="O28" t="s">
+        <v>63</v>
+      </c>
+      <c r="P28" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q28">
+        <v>28</v>
+      </c>
+      <c r="R28">
+        <v>19971024</v>
+      </c>
+      <c r="S28">
+        <v>0</v>
+      </c>
+      <c r="T28" s="1">
+        <v>44573</v>
+      </c>
+      <c r="U28" t="s">
+        <v>33</v>
+      </c>
+      <c r="V28" t="s">
+        <v>34</v>
+      </c>
+      <c r="W28">
+        <v>27.78257</v>
+      </c>
+      <c r="X28">
+        <v>70.070637000000005</v>
+      </c>
+      <c r="Y28">
+        <v>1</v>
+      </c>
+      <c r="Z28" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26">
+      <c r="A29" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" t="s">
+        <v>189</v>
+      </c>
+      <c r="C29" t="s">
+        <v>190</v>
+      </c>
+      <c r="D29" t="s">
+        <v>191</v>
+      </c>
+      <c r="E29">
+        <v>6</v>
+      </c>
+      <c r="F29">
+        <v>1003</v>
+      </c>
+      <c r="G29" t="s">
+        <v>28</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="J29" t="s">
+        <v>29</v>
+      </c>
+      <c r="K29">
+        <v>1</v>
+      </c>
+      <c r="L29" t="s">
+        <v>30</v>
+      </c>
+      <c r="M29" t="s">
+        <v>30</v>
+      </c>
+      <c r="N29" t="s">
+        <v>30</v>
+      </c>
+      <c r="O29" t="s">
+        <v>89</v>
+      </c>
+      <c r="P29" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q29">
+        <v>28</v>
+      </c>
+      <c r="R29">
+        <v>19900707</v>
+      </c>
+      <c r="S29">
+        <v>0</v>
+      </c>
+      <c r="T29" s="1">
+        <v>44573</v>
+      </c>
+      <c r="U29" t="s">
+        <v>33</v>
+      </c>
+      <c r="V29" t="s">
+        <v>34</v>
+      </c>
+      <c r="W29">
+        <v>28.055733</v>
+      </c>
+      <c r="X29">
+        <v>70.072055000000006</v>
+      </c>
+      <c r="Y29">
+        <v>1</v>
+      </c>
+      <c r="Z29" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26">
+      <c r="A30" t="s">
+        <v>24</v>
+      </c>
+      <c r="B30" t="s">
+        <v>192</v>
+      </c>
+      <c r="C30" t="s">
+        <v>193</v>
+      </c>
+      <c r="D30" t="s">
+        <v>194</v>
+      </c>
+      <c r="E30">
+        <v>4</v>
+      </c>
+      <c r="F30">
+        <v>1200</v>
+      </c>
+      <c r="G30" t="s">
+        <v>88</v>
+      </c>
+      <c r="H30">
+        <v>1</v>
+      </c>
+      <c r="J30" t="s">
+        <v>29</v>
+      </c>
+      <c r="K30">
+        <v>1</v>
+      </c>
+      <c r="L30" t="s">
+        <v>30</v>
+      </c>
+      <c r="M30" t="s">
+        <v>30</v>
+      </c>
+      <c r="N30" t="s">
+        <v>30</v>
+      </c>
+      <c r="O30" t="s">
+        <v>63</v>
+      </c>
+      <c r="P30" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q30">
+        <v>22</v>
+      </c>
+      <c r="R30">
+        <v>19990608</v>
+      </c>
+      <c r="S30">
+        <v>0</v>
+      </c>
+      <c r="T30" s="1">
+        <v>44573</v>
+      </c>
+      <c r="U30" t="s">
+        <v>33</v>
+      </c>
+      <c r="V30" t="s">
+        <v>34</v>
+      </c>
+      <c r="W30">
+        <v>27.705573000000001</v>
+      </c>
+      <c r="X30">
+        <v>70.074292</v>
+      </c>
+      <c r="Y30">
+        <v>1</v>
+      </c>
+      <c r="Z30" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26">
+      <c r="A31" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" t="s">
+        <v>192</v>
+      </c>
+      <c r="C31" t="s">
+        <v>193</v>
+      </c>
+      <c r="D31" t="s">
+        <v>194</v>
+      </c>
+      <c r="E31">
+        <v>4</v>
+      </c>
+      <c r="F31">
+        <v>1208</v>
+      </c>
+      <c r="G31" t="s">
+        <v>179</v>
+      </c>
+      <c r="H31">
+        <v>1</v>
+      </c>
+      <c r="J31" t="s">
+        <v>29</v>
+      </c>
+      <c r="K31">
+        <v>1</v>
+      </c>
+      <c r="L31" t="s">
+        <v>30</v>
+      </c>
+      <c r="M31" t="s">
+        <v>30</v>
+      </c>
+      <c r="N31" t="s">
+        <v>30</v>
+      </c>
+      <c r="O31" t="s">
+        <v>63</v>
+      </c>
+      <c r="P31" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q31">
+        <v>22</v>
+      </c>
+      <c r="R31">
+        <v>19990608</v>
+      </c>
+      <c r="S31">
+        <v>0</v>
+      </c>
+      <c r="T31" s="1">
+        <v>44573</v>
+      </c>
+      <c r="U31" t="s">
+        <v>33</v>
+      </c>
+      <c r="V31" t="s">
+        <v>34</v>
+      </c>
+      <c r="W31">
+        <v>27.705573000000001</v>
+      </c>
+      <c r="X31">
+        <v>70.074292</v>
+      </c>
+      <c r="Y31">
+        <v>1</v>
+      </c>
+      <c r="Z31" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26">
+      <c r="A32" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="E32" s="9">
+        <v>8</v>
+      </c>
+      <c r="F32" s="9">
+        <v>1001</v>
+      </c>
+      <c r="G32" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="H32" s="9">
+        <v>1</v>
+      </c>
+      <c r="I32" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J32" s="9"/>
+      <c r="K32" s="9">
+        <v>1</v>
+      </c>
+      <c r="L32" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="M32" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="N32" s="9">
+        <v>2189</v>
+      </c>
+      <c r="O32" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="P32" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q32" s="9">
+        <v>22</v>
+      </c>
+      <c r="R32" s="9">
+        <v>19891012</v>
+      </c>
+      <c r="S32" s="9">
+        <v>0</v>
+      </c>
+      <c r="T32" s="6">
+        <v>44573</v>
+      </c>
+      <c r="U32" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="V32" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="W32" s="9">
+        <v>24.938338000000002</v>
+      </c>
+      <c r="X32" s="9">
+        <v>69.426393000000004</v>
+      </c>
+      <c r="Y32" s="9">
+        <v>1</v>
+      </c>
+      <c r="Z32" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="33" spans="1:26">
+      <c r="A33" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="E33" s="9">
+        <v>6</v>
+      </c>
+      <c r="F33" s="9">
+        <v>1003</v>
+      </c>
+      <c r="G33" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="H33" s="9">
+        <v>1</v>
+      </c>
+      <c r="I33" s="9"/>
+      <c r="J33" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="K33" s="9">
+        <v>1</v>
+      </c>
+      <c r="L33" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="M33" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="N33" s="9">
+        <v>2189</v>
+      </c>
+      <c r="O33" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="P33" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q33" s="9">
+        <v>22</v>
+      </c>
+      <c r="R33" s="9">
+        <v>20020706</v>
+      </c>
+      <c r="S33" s="9">
+        <v>0</v>
+      </c>
+      <c r="T33" s="6">
+        <v>44573</v>
+      </c>
+      <c r="U33" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="V33" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="W33" s="9">
+        <v>24.938338000000002</v>
+      </c>
+      <c r="X33" s="9">
+        <v>69.426393000000004</v>
+      </c>
+      <c r="Y33" s="9">
+        <v>1</v>
+      </c>
+      <c r="Z33" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="34" spans="1:26">
+      <c r="A34" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E34" s="9">
+        <v>8</v>
+      </c>
+      <c r="F34" s="9">
+        <v>1001</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="H34" s="9">
+        <v>0</v>
+      </c>
+      <c r="I34" s="9"/>
+      <c r="J34" s="9"/>
+      <c r="K34" s="9">
+        <v>1</v>
+      </c>
+      <c r="L34" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="M34" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="N34" s="9">
+        <v>2185</v>
+      </c>
+      <c r="O34" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="P34" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q34" s="9">
+        <v>22</v>
+      </c>
+      <c r="R34" s="9">
+        <v>19730901</v>
+      </c>
+      <c r="S34" s="9">
+        <v>19891013</v>
+      </c>
+      <c r="T34" s="6">
+        <v>44573</v>
+      </c>
+      <c r="U34" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="V34" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="W34" s="9">
+        <v>24.945211</v>
+      </c>
+      <c r="X34" s="9">
+        <v>69.427194</v>
+      </c>
+      <c r="Y34" s="9">
+        <v>1</v>
+      </c>
+      <c r="Z34" s="9" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="35" spans="1:26">
+      <c r="A35" t="s">
+        <v>24</v>
+      </c>
+      <c r="B35" t="s">
+        <v>142</v>
+      </c>
+      <c r="C35" t="s">
+        <v>143</v>
+      </c>
+      <c r="D35" t="s">
+        <v>144</v>
+      </c>
+      <c r="E35">
+        <v>3</v>
+      </c>
+      <c r="F35">
+        <v>2000</v>
+      </c>
+      <c r="G35" t="s">
+        <v>83</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="K35">
+        <v>0</v>
+      </c>
+      <c r="L35" t="s">
+        <v>30</v>
+      </c>
+      <c r="M35" t="s">
+        <v>30</v>
+      </c>
+      <c r="N35" t="s">
+        <v>30</v>
+      </c>
+      <c r="O35" t="s">
+        <v>145</v>
+      </c>
+      <c r="P35" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q35">
+        <v>22</v>
+      </c>
+      <c r="R35">
+        <v>0</v>
+      </c>
+      <c r="S35">
+        <v>0</v>
+      </c>
+      <c r="T35" s="1">
+        <v>44573</v>
+      </c>
+      <c r="U35" t="s">
+        <v>33</v>
+      </c>
+      <c r="V35" t="s">
+        <v>34</v>
+      </c>
+      <c r="W35">
+        <v>25.811848999999999</v>
+      </c>
+      <c r="X35">
+        <v>69.408237</v>
+      </c>
+      <c r="Y35">
+        <v>1</v>
+      </c>
+      <c r="Z35" s="13" t="s">
+        <v>274</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:Z34" xr:uid="{9F911D2C-4B8B-480B-A44B-36F3EB2E8744}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Z34">
+      <sortCondition ref="D1:D34"/>
+    </sortState>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Z34">
+    <sortCondition ref="A1"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>